<commit_message>
pre jounral format MS
</commit_message>
<xml_diff>
--- a/data/Coregonine-Temperature-Experiment-AdultMeasurements.xlsx
+++ b/data/Coregonine-Temperature-Experiment-AdultMeasurements.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylor/SynologyDrive/Cisco-Climate-Change/Coregonine-Latitude-Embryo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF49FE2-2219-BC41-992D-98DEE6A188C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE7B12C2-4AD2-3C4B-99CC-CE20E32B22C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18620" yWindow="500" windowWidth="18200" windowHeight="19060" xr2:uid="{3E48306B-C0C5-BC40-9A7D-9108E98D2F1F}"/>
+    <workbookView xWindow="15400" yWindow="500" windowWidth="18200" windowHeight="19060" xr2:uid="{3E48306B-C0C5-BC40-9A7D-9108E98D2F1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <pivotCaches>
-    <pivotCache cacheId="4" r:id="rId2"/>
+    <pivotCache cacheId="1" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="14">
   <si>
     <t>Population</t>
   </si>
@@ -78,19 +78,7 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Row Labels</t>
-  </si>
-  <si>
-    <t>Min of TL</t>
-  </si>
-  <si>
-    <t>Total Min of TL</t>
-  </si>
-  <si>
-    <t>Total Max of TL</t>
-  </si>
-  <si>
-    <t>Max of TL</t>
+    <t>Average of FM</t>
   </si>
 </sst>
 </file>
@@ -126,12 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -258,7 +243,104 @@
       </sharedItems>
     </cacheField>
     <cacheField name="FM" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="9.6" maxValue="970"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="9.6" maxValue="970" count="96">
+        <n v="11.5"/>
+        <n v="25.9"/>
+        <n v="25"/>
+        <n v="24.1"/>
+        <n v="21"/>
+        <n v="13.5"/>
+        <n v="19.100000000000001"/>
+        <n v="11.2"/>
+        <n v="13.9"/>
+        <n v="15.9"/>
+        <n v="14.1"/>
+        <n v="13.2"/>
+        <n v="12"/>
+        <n v="18"/>
+        <n v="14"/>
+        <n v="16.899999999999999"/>
+        <n v="12.3"/>
+        <n v="13.6"/>
+        <n v="12.7"/>
+        <n v="9.6"/>
+        <n v="135.19999999999999"/>
+        <n v="108.5"/>
+        <n v="94.5"/>
+        <n v="141.30000000000001"/>
+        <n v="116.2"/>
+        <n v="129.6"/>
+        <n v="93.7"/>
+        <n v="202.2"/>
+        <n v="385.5"/>
+        <n v="130.30000000000001"/>
+        <n v="155.6"/>
+        <n v="279.3"/>
+        <n v="122.8"/>
+        <n v="218.2"/>
+        <n v="95.9"/>
+        <n v="90"/>
+        <n v="120.8"/>
+        <n v="122"/>
+        <n v="133.5"/>
+        <n v="654.5"/>
+        <n v="298.89999999999998"/>
+        <n v="776.9"/>
+        <n v="656.3"/>
+        <n v="612.1"/>
+        <n v="831.8"/>
+        <n v="882.4"/>
+        <n v="509.3"/>
+        <n v="970"/>
+        <n v="585.1"/>
+        <n v="579.20000000000005"/>
+        <n v="755.8"/>
+        <n v="644.1"/>
+        <n v="334.1"/>
+        <n v="433.2"/>
+        <n v="376.2"/>
+        <n v="660.3"/>
+        <n v="471.9"/>
+        <n v="542"/>
+        <n v="750"/>
+        <n v="719.7"/>
+        <n v="491"/>
+        <n v="582.9"/>
+        <n v="573.79999999999995"/>
+        <n v="359"/>
+        <n v="552.20000000000005"/>
+        <n v="573.70000000000005"/>
+        <n v="317"/>
+        <n v="635.29999999999995"/>
+        <n v="704"/>
+        <n v="469.6"/>
+        <n v="557.79999999999995"/>
+        <n v="795.8"/>
+        <n v="446.6"/>
+        <n v="646.79999999999995"/>
+        <n v="349.6"/>
+        <n v="563.4"/>
+        <n v="466.6"/>
+        <n v="616.79999999999995"/>
+        <n v="558.79999999999995"/>
+        <n v="355.1"/>
+        <n v="283"/>
+        <n v="280.5"/>
+        <n v="417.5"/>
+        <n v="510.9"/>
+        <n v="486.4"/>
+        <n v="640"/>
+        <n v="490"/>
+        <n v="525.20000000000005"/>
+        <n v="408.4"/>
+        <n v="340.2"/>
+        <n v="477.3"/>
+        <n v="454.3"/>
+        <n v="375.4"/>
+        <n v="440.2"/>
+        <n v="608.29999999999995"/>
+        <m/>
+      </sharedItems>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -276,686 +358,686 @@
     <x v="0"/>
     <n v="1"/>
     <x v="0"/>
-    <n v="11.5"/>
+    <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="2"/>
     <x v="1"/>
-    <n v="25.9"/>
+    <x v="1"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="3"/>
     <x v="2"/>
-    <n v="25"/>
+    <x v="2"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="4"/>
     <x v="3"/>
-    <n v="24.1"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="5"/>
     <x v="4"/>
-    <n v="21"/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="6"/>
     <x v="5"/>
-    <n v="13.5"/>
+    <x v="5"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="7"/>
     <x v="6"/>
-    <n v="19.100000000000001"/>
+    <x v="6"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="8"/>
     <x v="7"/>
-    <n v="11.2"/>
+    <x v="7"/>
   </r>
   <r>
     <x v="0"/>
     <x v="0"/>
     <n v="9"/>
     <x v="8"/>
-    <n v="13.9"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="1"/>
     <x v="6"/>
-    <n v="15.9"/>
+    <x v="9"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="2"/>
     <x v="8"/>
-    <n v="14.1"/>
+    <x v="10"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="3"/>
     <x v="9"/>
-    <n v="13.2"/>
+    <x v="11"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="4"/>
     <x v="10"/>
-    <n v="12"/>
+    <x v="12"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="5"/>
     <x v="11"/>
-    <n v="18"/>
+    <x v="13"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="6"/>
     <x v="12"/>
-    <n v="14"/>
+    <x v="14"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="7"/>
     <x v="6"/>
-    <n v="16.899999999999999"/>
+    <x v="15"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="8"/>
     <x v="13"/>
-    <n v="12.3"/>
+    <x v="16"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="9"/>
     <x v="14"/>
-    <n v="13.9"/>
+    <x v="8"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="10"/>
     <x v="9"/>
-    <n v="13.6"/>
+    <x v="17"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="11"/>
     <x v="15"/>
-    <n v="12.7"/>
+    <x v="18"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
     <n v="12"/>
     <x v="16"/>
-    <n v="9.6"/>
+    <x v="19"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="1"/>
     <x v="17"/>
-    <n v="135.19999999999999"/>
+    <x v="20"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="2"/>
     <x v="18"/>
-    <n v="108.5"/>
+    <x v="21"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="3"/>
     <x v="19"/>
-    <n v="94.5"/>
+    <x v="22"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="4"/>
     <x v="20"/>
-    <n v="141.30000000000001"/>
+    <x v="23"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="5"/>
     <x v="21"/>
-    <n v="116.2"/>
+    <x v="24"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="7"/>
     <x v="22"/>
-    <n v="129.6"/>
+    <x v="25"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
     <n v="8"/>
     <x v="18"/>
-    <n v="93.7"/>
+    <x v="26"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="1"/>
     <x v="23"/>
-    <n v="202.2"/>
+    <x v="27"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="2"/>
     <x v="24"/>
-    <n v="385.5"/>
+    <x v="28"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="3"/>
     <x v="25"/>
-    <n v="130.30000000000001"/>
+    <x v="29"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="4"/>
     <x v="26"/>
-    <n v="155.6"/>
+    <x v="30"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="5"/>
     <x v="27"/>
-    <n v="279.3"/>
+    <x v="31"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="6"/>
     <x v="22"/>
-    <n v="122.8"/>
+    <x v="32"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="7"/>
     <x v="28"/>
-    <n v="218.2"/>
+    <x v="33"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="8"/>
     <x v="29"/>
-    <n v="95.9"/>
+    <x v="34"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="9"/>
     <x v="29"/>
-    <n v="90"/>
+    <x v="35"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="10"/>
     <x v="30"/>
-    <n v="120.8"/>
+    <x v="36"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="11"/>
     <x v="31"/>
-    <n v="122"/>
+    <x v="37"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
     <n v="12"/>
     <x v="32"/>
-    <n v="133.5"/>
+    <x v="38"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="1"/>
     <x v="33"/>
-    <n v="654.5"/>
+    <x v="39"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="2"/>
     <x v="34"/>
-    <n v="298.89999999999998"/>
+    <x v="40"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="3"/>
     <x v="35"/>
-    <n v="776.9"/>
+    <x v="41"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="4"/>
     <x v="36"/>
-    <n v="656.3"/>
+    <x v="42"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="5"/>
     <x v="37"/>
-    <n v="612.1"/>
+    <x v="43"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="6"/>
     <x v="38"/>
-    <n v="831.8"/>
+    <x v="44"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="7"/>
     <x v="39"/>
-    <n v="882.4"/>
+    <x v="45"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="8"/>
     <x v="40"/>
-    <n v="509.3"/>
+    <x v="46"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="9"/>
     <x v="41"/>
-    <n v="970"/>
+    <x v="47"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="10"/>
     <x v="42"/>
-    <n v="585.1"/>
+    <x v="48"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="11"/>
     <x v="43"/>
-    <n v="579.20000000000005"/>
+    <x v="49"/>
   </r>
   <r>
     <x v="2"/>
     <x v="0"/>
     <n v="12"/>
     <x v="44"/>
-    <n v="755.8"/>
+    <x v="50"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="1"/>
     <x v="43"/>
-    <n v="644.1"/>
+    <x v="51"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="2"/>
     <x v="45"/>
-    <n v="334.1"/>
+    <x v="52"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="3"/>
     <x v="46"/>
-    <n v="433.2"/>
+    <x v="53"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="4"/>
     <x v="47"/>
-    <n v="376.2"/>
+    <x v="54"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="5"/>
     <x v="48"/>
-    <n v="660.3"/>
+    <x v="55"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="6"/>
     <x v="49"/>
-    <n v="471.9"/>
+    <x v="56"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="7"/>
     <x v="50"/>
-    <n v="542"/>
+    <x v="57"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="8"/>
     <x v="44"/>
-    <n v="750"/>
+    <x v="58"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="9"/>
     <x v="51"/>
-    <n v="719.7"/>
+    <x v="59"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="10"/>
     <x v="52"/>
-    <n v="491"/>
+    <x v="60"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="11"/>
     <x v="53"/>
-    <n v="582.9"/>
+    <x v="61"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="12"/>
     <x v="54"/>
-    <n v="573.79999999999995"/>
+    <x v="62"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="13"/>
     <x v="55"/>
-    <n v="359"/>
+    <x v="63"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="14"/>
     <x v="56"/>
-    <n v="552.20000000000005"/>
+    <x v="64"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="15"/>
     <x v="40"/>
-    <n v="573.70000000000005"/>
+    <x v="65"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
     <n v="16"/>
     <x v="57"/>
-    <n v="317"/>
+    <x v="66"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="1"/>
     <x v="56"/>
-    <n v="635.29999999999995"/>
+    <x v="67"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="2"/>
     <x v="54"/>
-    <n v="704"/>
+    <x v="68"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="3"/>
     <x v="58"/>
-    <n v="469.6"/>
+    <x v="69"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="4"/>
     <x v="59"/>
-    <n v="557.79999999999995"/>
+    <x v="70"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="5"/>
     <x v="60"/>
-    <n v="795.8"/>
+    <x v="71"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="6"/>
     <x v="55"/>
-    <n v="446.6"/>
+    <x v="72"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="7"/>
     <x v="61"/>
-    <n v="646.79999999999995"/>
+    <x v="73"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="8"/>
     <x v="62"/>
-    <n v="349.6"/>
+    <x v="74"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="9"/>
     <x v="63"/>
-    <n v="563.4"/>
+    <x v="75"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="10"/>
     <x v="64"/>
-    <n v="466.6"/>
+    <x v="76"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="11"/>
     <x v="56"/>
-    <n v="616.79999999999995"/>
+    <x v="77"/>
   </r>
   <r>
     <x v="3"/>
     <x v="0"/>
     <n v="12"/>
     <x v="65"/>
-    <n v="558.79999999999995"/>
+    <x v="78"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="1"/>
     <x v="62"/>
-    <n v="355.1"/>
+    <x v="79"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="2"/>
     <x v="66"/>
-    <n v="283"/>
+    <x v="80"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="3"/>
     <x v="67"/>
-    <n v="280.5"/>
+    <x v="81"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="4"/>
     <x v="68"/>
-    <n v="417.5"/>
+    <x v="82"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="5"/>
     <x v="69"/>
-    <n v="510.9"/>
+    <x v="83"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="6"/>
     <x v="70"/>
-    <n v="486.4"/>
+    <x v="84"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="7"/>
     <x v="71"/>
-    <n v="640"/>
+    <x v="85"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="8"/>
     <x v="72"/>
-    <n v="490"/>
+    <x v="86"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="9"/>
     <x v="73"/>
-    <n v="525.20000000000005"/>
+    <x v="87"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="10"/>
     <x v="74"/>
-    <n v="408.4"/>
+    <x v="88"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="11"/>
     <x v="57"/>
-    <n v="340.2"/>
+    <x v="89"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="12"/>
     <x v="63"/>
-    <n v="477.3"/>
+    <x v="90"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="13"/>
     <x v="75"/>
-    <n v="454.3"/>
+    <x v="91"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="14"/>
     <x v="74"/>
-    <n v="375.4"/>
+    <x v="92"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="15"/>
     <x v="76"/>
-    <n v="440.2"/>
+    <x v="93"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
     <n v="16"/>
     <x v="61"/>
-    <n v="608.29999999999995"/>
+    <x v="94"/>
   </r>
   <r>
     <x v="4"/>
     <x v="2"/>
     <m/>
     <x v="77"/>
-    <m/>
+    <x v="95"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD37B30F-0408-7341-A805-CBACA7158804}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="G1:M6" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BD37B30F-0408-7341-A805-CBACA7158804}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="G1:J3" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField axis="axisCol" showAll="0">
       <items count="6">
@@ -967,7 +1049,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField showAll="0">
       <items count="4">
         <item x="0"/>
         <item x="1"/>
@@ -976,7 +1058,7 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
+    <pivotField showAll="0">
       <items count="79">
         <item x="7"/>
         <item x="16"/>
@@ -1059,51 +1141,127 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="97">
+        <item x="19"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="12"/>
+        <item x="16"/>
+        <item x="18"/>
+        <item x="11"/>
+        <item x="5"/>
+        <item x="17"/>
+        <item x="8"/>
+        <item x="14"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="15"/>
+        <item x="13"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="35"/>
+        <item x="26"/>
+        <item x="22"/>
+        <item x="34"/>
+        <item x="21"/>
+        <item x="24"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="32"/>
+        <item x="25"/>
+        <item x="29"/>
+        <item x="38"/>
+        <item x="20"/>
+        <item x="23"/>
+        <item x="30"/>
+        <item x="27"/>
+        <item x="33"/>
+        <item x="31"/>
+        <item x="81"/>
+        <item x="80"/>
+        <item x="40"/>
+        <item x="66"/>
+        <item x="52"/>
+        <item x="89"/>
+        <item x="74"/>
+        <item x="79"/>
+        <item x="63"/>
+        <item x="92"/>
+        <item x="54"/>
+        <item x="28"/>
+        <item x="88"/>
+        <item x="82"/>
+        <item x="53"/>
+        <item x="93"/>
+        <item x="72"/>
+        <item x="91"/>
+        <item x="76"/>
+        <item x="69"/>
+        <item x="56"/>
+        <item x="90"/>
+        <item x="84"/>
+        <item x="86"/>
+        <item x="60"/>
+        <item x="46"/>
+        <item x="83"/>
+        <item x="87"/>
+        <item x="57"/>
+        <item x="64"/>
+        <item x="70"/>
+        <item x="78"/>
+        <item x="75"/>
+        <item x="65"/>
+        <item x="62"/>
+        <item x="49"/>
+        <item x="61"/>
+        <item x="48"/>
+        <item x="94"/>
+        <item x="43"/>
+        <item x="77"/>
+        <item x="67"/>
+        <item x="85"/>
+        <item x="51"/>
+        <item x="73"/>
+        <item x="39"/>
+        <item x="42"/>
+        <item x="55"/>
+        <item x="68"/>
+        <item x="59"/>
+        <item x="58"/>
+        <item x="50"/>
+        <item x="41"/>
+        <item x="71"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item x="47"/>
+        <item x="95"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="3">
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="3">
     <i>
-      <x/>
+      <x v="2"/>
     </i>
     <i>
-      <x v="1"/>
+      <x v="3"/>
     </i>
     <i t="grand">
       <x/>
     </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="0"/>
-    <field x="-2"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x v="2"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-      <x/>
-    </i>
-    <i r="1" i="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-    <i t="grand" i="1">
-      <x/>
-    </i>
   </colItems>
-  <dataFields count="2">
-    <dataField name="Min of TL" fld="3" subtotal="min" baseField="0" baseItem="0"/>
-    <dataField name="Max of TL" fld="3" subtotal="max" baseField="0" baseItem="0"/>
+  <dataFields count="1">
+    <dataField name="Average of FM" fld="4" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -1414,10 +1572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E38C00-8BCC-C44F-9CD1-57696D1BBA15}">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1427,22 +1585,21 @@
     <col min="3" max="3" width="3.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1462,7 +1619,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1481,17 +1638,14 @@
       <c r="H2" t="s">
         <v>10</v>
       </c>
+      <c r="I2" t="s">
+        <v>9</v>
+      </c>
       <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1507,23 +1661,20 @@
       <c r="E3">
         <v>25.9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" t="s">
-        <v>14</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H3" s="2">
+        <v>496.56428571428563</v>
+      </c>
+      <c r="I3" s="2">
+        <v>589.04999999999995</v>
+      </c>
+      <c r="J3" s="2">
+        <v>542.80714285714282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1539,29 +1690,8 @@
       <c r="E4">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="3">
-        <v>347</v>
-      </c>
-      <c r="I4" s="3">
-        <v>425</v>
-      </c>
-      <c r="J4" s="3">
-        <v>326</v>
-      </c>
-      <c r="K4" s="3">
-        <v>503</v>
-      </c>
-      <c r="L4" s="3">
-        <v>326</v>
-      </c>
-      <c r="M4" s="3">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1577,29 +1707,8 @@
       <c r="E5">
         <v>24.1</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3">
-        <v>321</v>
-      </c>
-      <c r="I5" s="3">
-        <v>415</v>
-      </c>
-      <c r="J5" s="3">
-        <v>343</v>
-      </c>
-      <c r="K5" s="3">
-        <v>463</v>
-      </c>
-      <c r="L5" s="3">
-        <v>321</v>
-      </c>
-      <c r="M5" s="3">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1615,29 +1724,8 @@
       <c r="E6">
         <v>21</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="3">
-        <v>321</v>
-      </c>
-      <c r="I6" s="3">
-        <v>425</v>
-      </c>
-      <c r="J6" s="3">
-        <v>326</v>
-      </c>
-      <c r="K6" s="3">
-        <v>503</v>
-      </c>
-      <c r="L6" s="3">
-        <v>321</v>
-      </c>
-      <c r="M6" s="3">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -1654,7 +1742,7 @@
         <v>13.5</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1671,7 +1759,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1688,7 +1776,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -1705,7 +1793,7 @@
         <v>13.9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -1722,7 +1810,7 @@
         <v>15.9</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +1827,7 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -1756,7 +1844,7 @@
         <v>13.2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -1773,7 +1861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -1790,7 +1878,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>1</v>
       </c>

</xml_diff>